<commit_message>
update Economy 2008 python model
</commit_message>
<xml_diff>
--- a/Examples/ANP_USEconomy_Prediction2008/2008Economy_filled.xlsx
+++ b/Examples/ANP_USEconomy_Prediction2008/2008Economy_filled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubCode\AhpAnpLib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/ANP_USEconomy_Prediction2008/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DBDC50A-0E0D-4AA0-9C94-BD5481C601DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626591F-3EEE-284D-A12D-418B87831BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="9000" windowWidth="20920" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise_comp" sheetId="1" r:id="rId1"/>
@@ -333,9 +333,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,9 +373,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,9 +408,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,9 +460,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -621,26 +655,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="H260" sqref="H260"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.68359375" customWidth="1"/>
+    <col min="1" max="21" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -669,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -696,7 +730,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -720,14 +754,15 @@
         <v>0.125</v>
       </c>
       <c r="G5" s="6">
-        <v>7</v>
+        <f>1/7</f>
+        <v>0.14285714285714285</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -759,7 +794,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -791,7 +826,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -822,7 +857,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -832,7 +867,7 @@
       </c>
       <c r="C9" s="8">
         <f>1/G5</f>
-        <v>0.14285714285714285</v>
+        <v>7</v>
       </c>
       <c r="D9" s="8">
         <f>1/G6</f>
@@ -854,7 +889,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -887,17 +922,17 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -923,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -952,7 +987,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -981,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1010,12 +1045,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1035,7 +1070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1111,7 @@
         <v>0.16666700000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
@@ -1119,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1159,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1242,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1267,17 +1302,17 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="31" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
@@ -1309,7 +1344,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
@@ -1342,7 +1377,7 @@
         <v>0.14285700000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>24</v>
       </c>
@@ -1376,7 +1411,7 @@
         <v>0.14285700000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
@@ -1411,7 +1446,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
@@ -1447,12 +1482,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
@@ -1469,7 +1504,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
@@ -1504,7 +1539,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1572,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>24</v>
       </c>
@@ -1571,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>25</v>
       </c>
@@ -1606,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>26</v>
       </c>
@@ -1627,17 +1662,17 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="49" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>22</v>
       </c>
@@ -1669,7 +1704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1702,7 +1737,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1736,7 +1771,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>25</v>
       </c>
@@ -1771,7 +1806,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>26</v>
       </c>
@@ -1807,12 +1842,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +1864,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>22</v>
       </c>
@@ -1864,7 +1899,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>23</v>
       </c>
@@ -1897,7 +1932,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>24</v>
       </c>
@@ -1931,7 +1966,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>26</v>
       </c>
@@ -1987,17 +2022,17 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="67" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +2046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>27</v>
       </c>
@@ -2024,7 +2059,7 @@
       </c>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>28</v>
       </c>
@@ -2037,12 +2072,12 @@
       </c>
       <c r="D71" s="7"/>
     </row>
-    <row r="74" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>1</v>
       </c>
@@ -2059,7 +2094,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
@@ -2094,7 +2129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>24</v>
       </c>
@@ -2161,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>25</v>
       </c>
@@ -2196,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>26</v>
       </c>
@@ -2217,12 +2252,12 @@
       </c>
       <c r="F80" s="7"/>
     </row>
-    <row r="83" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +2274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>22</v>
       </c>
@@ -2274,7 +2309,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>23</v>
       </c>
@@ -2307,7 +2342,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>24</v>
       </c>
@@ -2341,7 +2376,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>26</v>
       </c>
@@ -2397,12 +2432,12 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="92" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
@@ -2419,7 +2454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>22</v>
       </c>
@@ -2454,7 +2489,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2522,7 @@
         <v>0.33329999999999899</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>24</v>
       </c>
@@ -2521,7 +2556,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>25</v>
       </c>
@@ -2556,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>26</v>
       </c>
@@ -2577,12 +2612,12 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="101" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>1</v>
       </c>
@@ -2599,7 +2634,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>22</v>
       </c>
@@ -2634,7 +2669,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>23</v>
       </c>
@@ -2667,7 +2702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>24</v>
       </c>
@@ -2701,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>25</v>
       </c>
@@ -2736,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>26</v>
       </c>
@@ -2757,12 +2792,12 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="110" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>1</v>
       </c>
@@ -2779,7 +2814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>22</v>
       </c>
@@ -2814,7 +2849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>23</v>
       </c>
@@ -2847,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>24</v>
       </c>
@@ -2881,7 +2916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>25</v>
       </c>
@@ -2916,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>26</v>
       </c>
@@ -2937,12 +2972,12 @@
       </c>
       <c r="F116" s="7"/>
     </row>
-    <row r="119" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>1</v>
       </c>
@@ -2959,7 +2994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +3029,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>23</v>
       </c>
@@ -3027,7 +3062,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>24</v>
       </c>
@@ -3061,7 +3096,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>25</v>
       </c>
@@ -3096,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>26</v>
       </c>
@@ -3117,12 +3152,12 @@
       </c>
       <c r="F125" s="7"/>
     </row>
-    <row r="128" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>1</v>
       </c>
@@ -3139,7 +3174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>22</v>
       </c>
@@ -3174,7 +3209,7 @@
         <v>0.14285700000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>23</v>
       </c>
@@ -3207,7 +3242,7 @@
         <v>0.16666700000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>24</v>
       </c>
@@ -3241,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>25</v>
       </c>
@@ -3276,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>26</v>
       </c>
@@ -3297,17 +3332,17 @@
       </c>
       <c r="F134" s="7"/>
     </row>
-    <row r="137" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>22</v>
       </c>
@@ -3339,7 +3374,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>23</v>
       </c>
@@ -3372,7 +3407,7 @@
         <v>0.14285700000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>24</v>
       </c>
@@ -3406,7 +3441,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>25</v>
       </c>
@@ -3441,7 +3476,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>26</v>
       </c>
@@ -3477,17 +3512,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>22</v>
       </c>
@@ -3519,7 +3554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>23</v>
       </c>
@@ -3552,7 +3587,7 @@
         <v>0.14285700000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>24</v>
       </c>
@@ -3586,7 +3621,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>25</v>
       </c>
@@ -3621,7 +3656,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>26</v>
       </c>
@@ -3657,17 +3692,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>29</v>
       </c>
@@ -3705,7 +3740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>30</v>
       </c>
@@ -3744,7 +3779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>31</v>
       </c>
@@ -3784,7 +3819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>32</v>
       </c>
@@ -3825,7 +3860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>33</v>
       </c>
@@ -3867,7 +3902,7 @@
         <v>0.33329999999999899</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>34</v>
       </c>
@@ -3910,17 +3945,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>22</v>
       </c>
@@ -3952,7 +3987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>23</v>
       </c>
@@ -3985,7 +4020,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>24</v>
       </c>
@@ -4019,7 +4054,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>25</v>
       </c>
@@ -4054,7 +4089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>26</v>
       </c>
@@ -4090,17 +4125,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>22</v>
       </c>
@@ -4132,7 +4167,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>23</v>
       </c>
@@ -4165,7 +4200,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>24</v>
       </c>
@@ -4199,7 +4234,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>25</v>
       </c>
@@ -4234,7 +4269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>26</v>
       </c>
@@ -4270,17 +4305,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>22</v>
       </c>
@@ -4312,7 +4347,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>23</v>
       </c>
@@ -4345,7 +4380,7 @@
         <v>0.16666700000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>24</v>
       </c>
@@ -4379,7 +4414,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>25</v>
       </c>
@@ -4414,7 +4449,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>26</v>
       </c>
@@ -4450,17 +4485,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>22</v>
       </c>
@@ -4492,7 +4527,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>23</v>
       </c>
@@ -4525,7 +4560,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>24</v>
       </c>
@@ -4559,7 +4594,7 @@
         <v>0.33333299999999899</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>25</v>
       </c>
@@ -4594,7 +4629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>26</v>
       </c>
@@ -4630,17 +4665,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>22</v>
       </c>
@@ -4672,7 +4707,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>23</v>
       </c>
@@ -4705,7 +4740,7 @@
         <v>0.194746</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>24</v>
       </c>
@@ -4739,7 +4774,7 @@
         <v>0.458484</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>25</v>
       </c>
@@ -4774,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>26</v>
       </c>
@@ -4810,17 +4845,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>22</v>
       </c>
@@ -4852,7 +4887,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
         <v>23</v>
       </c>
@@ -4885,7 +4920,7 @@
         <v>0.194747</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>24</v>
       </c>
@@ -4919,7 +4954,7 @@
         <v>0.45847700000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>25</v>
       </c>
@@ -4954,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>26</v>
       </c>
@@ -4990,17 +5025,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>22</v>
       </c>
@@ -5032,7 +5067,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
         <v>23</v>
       </c>
@@ -5065,7 +5100,7 @@
         <v>0.194746</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
         <v>24</v>
       </c>
@@ -5099,7 +5134,7 @@
         <v>0.458484</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>25</v>
       </c>
@@ -5134,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
         <v>26</v>
       </c>
@@ -5170,17 +5205,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>35</v>
       </c>
@@ -5206,7 +5241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
         <v>0</v>
       </c>
@@ -5233,7 +5268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
         <v>11</v>
       </c>
@@ -5261,7 +5296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>16</v>
       </c>
@@ -5290,17 +5325,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>35</v>
       </c>
@@ -5326,7 +5361,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
         <v>0</v>
       </c>
@@ -5353,7 +5388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>11</v>
       </c>
@@ -5381,7 +5416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
         <v>16</v>
       </c>
@@ -5410,17 +5445,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>35</v>
       </c>
@@ -5446,7 +5481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
         <v>0</v>
       </c>
@@ -5473,7 +5508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>11</v>
       </c>
@@ -5501,7 +5536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
         <v>16</v>
       </c>
@@ -5530,17 +5565,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>35</v>
       </c>
@@ -5566,7 +5601,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
         <v>0</v>
       </c>
@@ -5593,7 +5628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
         <v>11</v>
       </c>
@@ -5621,7 +5656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>